<commit_message>
Updated docs and panel
</commit_message>
<xml_diff>
--- a/IO.xlsx
+++ b/IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MosaicApp\SPSZL-PLC-Zakladac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MosaicApp\SinZakladac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C54378-242D-4BA7-AC19-A815FF7B46CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA64F40B-057A-48DB-88B8-F5AC193B7C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{64A97B4D-A654-4124-AB1E-FD2AD8762B5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64A97B4D-A654-4124-AB1E-FD2AD8762B5D}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1367,21 +1367,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51600EDD-51B9-4B52-9D26-A35A9565580D}">
   <dimension ref="B1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H40" sqref="B37:H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -1423,7 +1423,7 @@
       <c r="G3" s="61"/>
       <c r="H3" s="42"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="G4" s="62"/>
       <c r="H4" s="43"/>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="37">
         <v>3</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="G5" s="63"/>
       <c r="H5" s="44"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <v>4</v>
       </c>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="H6" s="45"/>
     </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="15">
         <v>5</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="17">
         <v>6</v>
       </c>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="H8" s="47"/>
     </row>
-    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19">
         <v>7</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="H9" s="48"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="21">
         <v>8</v>
       </c>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="H10" s="49"/>
     </row>
-    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23">
         <v>9</v>
       </c>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="H11" s="50"/>
     </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="21">
         <v>11</v>
       </c>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="H13" s="49"/>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="23">
         <v>12</v>
       </c>
@@ -1640,7 +1640,7 @@
       </c>
       <c r="H14" s="50"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="31">
         <v>13</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="33">
         <v>14</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="33">
         <v>15</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="33">
         <v>16</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="35">
         <v>17</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="25">
         <v>18</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="13">
         <v>25</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="27">
         <v>26</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="27">
         <v>27</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="27">
         <v>28</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15">
         <v>29</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <v>30</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="29">
         <v>31</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="29">
         <v>32</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="29">
         <v>33</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="19">
         <v>34</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="9">
         <v>35</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>36</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="21">
         <v>37</v>
       </c>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="H33" s="49"/>
     </row>
-    <row r="34" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="23">
         <v>38</v>
       </c>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="H34" s="50"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="31">
         <v>39</v>
       </c>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="H35" s="52"/>
     </row>
-    <row r="36" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="35">
         <v>40</v>
       </c>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="H36" s="54"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>-1</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>-1</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>-1</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>-1</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>-1</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>-1</v>
       </c>

</xml_diff>